<commit_message>
ErrorMSG excel tábla létrehozva, egyedi és egységes hibaüzenetek dokumentálásának megkezdése, későbbiekben bővítendő.
</commit_message>
<xml_diff>
--- a/testDoksi.xlsx
+++ b/testDoksi.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dariu\Desktop\Erettsegizzunk-Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernát Olivér\Desktop\doski\Erettsegizzunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BC2049-BC2F-4326-A210-A61C41D6B584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B06974-6B56-49FF-AC85-6514545B159B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Docs" sheetId="5" r:id="rId1"/>
-    <sheet name="test_page_title" sheetId="1" r:id="rId2"/>
-    <sheet name="test_element_presence" sheetId="2" r:id="rId3"/>
-    <sheet name="test_navigation" sheetId="3" r:id="rId4"/>
-    <sheet name="test_function" sheetId="4" r:id="rId5"/>
+    <sheet name="ErrorMSG" sheetId="6" r:id="rId2"/>
+    <sheet name="test_page_title" sheetId="1" r:id="rId3"/>
+    <sheet name="test_element_presence" sheetId="2" r:id="rId4"/>
+    <sheet name="test_navigation" sheetId="3" r:id="rId5"/>
+    <sheet name="test_function" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="90">
   <si>
     <t>Teszt lépés</t>
   </si>
@@ -186,13 +187,127 @@
   </si>
   <si>
     <t>5.58s</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Az elem nem található</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>GetFeladatoks</t>
+  </si>
+  <si>
+    <t>Hiba történt az adatok lekérdezése közben</t>
+  </si>
+  <si>
+    <t>GetFeladatoksTipusSzint</t>
+  </si>
+  <si>
+    <t>A keresési feltétel nem lehet üres</t>
+  </si>
+  <si>
+    <t>A keresett adat nem található</t>
+  </si>
+  <si>
+    <t>GetFeladat</t>
+  </si>
+  <si>
+    <t>PutFeladatok</t>
+  </si>
+  <si>
+    <t>Hozzáférés megtagadva</t>
+  </si>
+  <si>
+    <t>Helytelen azonosító</t>
+  </si>
+  <si>
+    <t>Hiba történt az adatok mentése közben</t>
+  </si>
+  <si>
+    <t>PostFeladat</t>
+  </si>
+  <si>
+    <t>PostFeladatok</t>
+  </si>
+  <si>
+    <t>A feltöltendő adat nem lehet üres</t>
+  </si>
+  <si>
+    <t>DeleteFeladatok</t>
+  </si>
+  <si>
+    <t>Hiba történt az adatok törlése közben</t>
+  </si>
+  <si>
+    <t>Törlendő adat nem található</t>
+  </si>
+  <si>
+    <t>Kapcsolati hiba</t>
+  </si>
+  <si>
+    <t>Hibás név, jelszó páros</t>
+  </si>
+  <si>
+    <t>SaltRequest</t>
+  </si>
+  <si>
+    <t>Hiba történt a bejelentkezés során</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Registry</t>
+  </si>
+  <si>
+    <t>Hiba történt a regisztráció során</t>
+  </si>
+  <si>
+    <t>EndOfTheRegistry</t>
+  </si>
+  <si>
+    <t>GetTantargyak</t>
+  </si>
+  <si>
+    <t>PostTantargyak</t>
+  </si>
+  <si>
+    <t>PutTantargyak</t>
+  </si>
+  <si>
+    <t>DeleteTantargyak</t>
+  </si>
+  <si>
+    <t>GetFelhasznalok</t>
+  </si>
+  <si>
+    <t>GetKorlevel</t>
+  </si>
+  <si>
+    <t>PutFelhasznalok</t>
+  </si>
+  <si>
+    <t>DeleteFelhasznalok</t>
+  </si>
+  <si>
+    <t>Api errorMSG</t>
+  </si>
+  <si>
+    <t>Admin errorMSG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,13 +322,47 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -243,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -252,6 +401,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,21 +694,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5FF267-F947-44FF-9106-CA6185654F98}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -566,7 +725,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -583,7 +742,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -600,7 +759,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -617,7 +776,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -640,6 +799,1180 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D487B678-5BA6-44EE-BB72-0A61B2EBDFBA}">
+  <dimension ref="A1:C133"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="80.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>18</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>25</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>26</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>27</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>28</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>29</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
+        <v>30</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="6">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="6">
+        <v>32</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="6">
+        <v>33</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>34</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>35</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
+        <v>36</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>38</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
+        <v>39</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>40</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="6">
+        <v>41</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>42</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>43</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
+        <v>44</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="11">
+        <v>45</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
+        <v>46</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="6">
+        <v>48</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="6">
+        <v>49</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="11">
+        <v>50</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
+        <v>51</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="7">
+        <v>52</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="11">
+        <v>53</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="6">
+        <v>54</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="6">
+        <v>55</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="11">
+        <v>56</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="6">
+        <v>57</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="7">
+        <v>58</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="11">
+        <v>59</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="6">
+        <v>60</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="6">
+        <v>61</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="11">
+        <v>62</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="7">
+        <v>63</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="6">
+        <v>64</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="11">
+        <v>65</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="6">
+        <v>66</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="11">
+        <v>68</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="6">
+        <v>69</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="7">
+        <v>70</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="11">
+        <v>71</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="6">
+        <v>72</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="6">
+        <v>73</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="6">
+        <v>74</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="7">
+        <v>75</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="6">
+        <v>76</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="6">
+        <v>77</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="6">
+        <v>78</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="11">
+        <v>79</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="6">
+        <v>80</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="6"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="11"/>
+    </row>
+    <row r="84" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="6"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="11"/>
+    </row>
+    <row r="85" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="11"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="11"/>
+    </row>
+    <row r="86" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="6"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+    </row>
+    <row r="87" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="6"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+    </row>
+    <row r="89" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="11"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+    </row>
+    <row r="90" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="6"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+    </row>
+    <row r="91" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="6"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+    </row>
+    <row r="92" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="6"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+    </row>
+    <row r="93" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="11"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+    </row>
+    <row r="94" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="6"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+    </row>
+    <row r="95" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="6"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+    </row>
+    <row r="100" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A100" s="9"/>
+      <c r="B100" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C100" s="9"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="5">
+        <v>500</v>
+      </c>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="5">
+        <v>501</v>
+      </c>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="5"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="5"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="5"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="5"/>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="5"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="5"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="5"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="5"/>
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="5"/>
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="5"/>
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="5"/>
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="5"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="5"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="5"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="5"/>
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="5"/>
+      <c r="B118" s="5"/>
+      <c r="C118" s="5"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="5"/>
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="5"/>
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="5"/>
+      <c r="B121" s="5"/>
+      <c r="C121" s="5"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="5"/>
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="5"/>
+      <c r="B123" s="5"/>
+      <c r="C123" s="5"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="5"/>
+      <c r="B124" s="5"/>
+      <c r="C124" s="5"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="5"/>
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="5"/>
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="5"/>
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="5"/>
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="5"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="5"/>
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="5"/>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="5"/>
+      <c r="B133" s="5"/>
+      <c r="C133" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -647,16 +1980,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -670,7 +2003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -684,7 +2017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -702,7 +2035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7591F0D7-29BF-434D-9D48-85DDD91AD0D5}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -710,16 +2043,16 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="37.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -733,7 +2066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -747,7 +2080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -759,7 +2092,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -776,7 +2109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09277DF6-3E9C-472A-A761-D842BEF4921B}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -784,16 +2117,16 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -807,7 +2140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -821,7 +2154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -833,7 +2166,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -850,7 +2183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366C0304-8F71-4FA9-8DE7-2CE4C3CFD20A}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -858,16 +2191,16 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -881,7 +2214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -895,7 +2228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -909,7 +2242,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -921,7 +2254,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -935,7 +2268,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -947,7 +2280,7 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -961,7 +2294,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
@@ -973,7 +2306,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -987,7 +2320,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -999,7 +2332,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Statisztika hibaüzenetek javítása / átírása
</commit_message>
<xml_diff>
--- a/testDoksi.xlsx
+++ b/testDoksi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernát Olivér\Desktop\doski\Erettsegizzunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35D1157-65A4-44D3-AEF1-6F4AD40B582E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4241A8F-69BD-4AC6-85C9-2F374A11275C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="131">
   <si>
     <t>Teszt lépés</t>
   </si>
@@ -402,22 +402,28 @@
     <t>ElfelejtettJelszo</t>
   </si>
   <si>
-    <t>GetUserStatistic</t>
-  </si>
-  <si>
-    <t>PutUserStatistic</t>
-  </si>
-  <si>
-    <t>GetUserStatistics</t>
+    <t>CheckCaptcha</t>
+  </si>
+  <si>
+    <t>A keresett adatok nem találhatóak</t>
+  </si>
+  <si>
+    <t>GetMatchHistory</t>
+  </si>
+  <si>
+    <t>GetStatisticsDeatiled</t>
+  </si>
+  <si>
+    <t>GetTaskFilloutCount</t>
   </si>
   <si>
     <t>PostUserStatistic</t>
   </si>
   <si>
-    <t>CheckCaptcha</t>
-  </si>
-  <si>
-    <t>A keresett adatok nem találhatóak</t>
+    <t>GetFillingByDate</t>
+  </si>
+  <si>
+    <t>DeleteUserStatistic</t>
   </si>
 </sst>
 </file>
@@ -1020,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D487B678-5BA6-44EE-BB72-0A61B2EBDFBA}">
   <dimension ref="A1:C231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2210,7 +2216,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>115</v>
@@ -2246,7 +2252,7 @@
         <v>121</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -2257,7 +2263,7 @@
         <v>120</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -2323,7 +2329,7 @@
         <v>63</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -2331,10 +2337,10 @@
         <v>117</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -2342,10 +2348,10 @@
         <v>118</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -2353,10 +2359,10 @@
         <v>119</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -2364,10 +2370,10 @@
         <v>120</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -2375,10 +2381,10 @@
         <v>121</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -2386,10 +2392,10 @@
         <v>122</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -2400,7 +2406,7 @@
         <v>72</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -2411,7 +2417,7 @@
         <v>65</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -2419,10 +2425,10 @@
         <v>125</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -2430,10 +2436,10 @@
         <v>126</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -2441,10 +2447,10 @@
         <v>127</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -2452,10 +2458,10 @@
         <v>128</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -2463,10 +2469,10 @@
         <v>129</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -2477,7 +2483,7 @@
         <v>72</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -2488,7 +2494,7 @@
         <v>65</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -2496,10 +2502,10 @@
         <v>132</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -2517,22 +2523,34 @@
       <c r="A136" s="6">
         <v>134</v>
       </c>
-      <c r="B136" s="6"/>
-      <c r="C136" s="6"/>
+      <c r="B136" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="6">
         <v>135</v>
       </c>
-      <c r="B137" s="6"/>
-      <c r="C137" s="6"/>
+      <c r="B137" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="6">
         <v>136</v>
       </c>
-      <c r="B138" s="6"/>
-      <c r="C138" s="6"/>
+      <c r="B138" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="6">

</xml_diff>